<commit_message>
fix(quiz): guard against empty word rows from imported data
</commit_message>
<xml_diff>
--- a/public/storyassets/story_words.xlsx
+++ b/public/storyassets/story_words.xlsx
@@ -1556,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3280,26 +3280,6 @@
         <v>388</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>62</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>